<commit_message>
renamed testing data and plotted all graphs
</commit_message>
<xml_diff>
--- a/CouponData/Coupon ID DataSheet.xlsx
+++ b/CouponData/Coupon ID DataSheet.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saschastevens/Desktop/SurfURS/CouponData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\SurfboardProj\SurfURS\CouponData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E23637B-F294-8A4C-9BA0-B8D40485D362}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07EF696A-A775-4479-A446-83D0BB89D987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1060" windowWidth="28040" windowHeight="16280" xr2:uid="{D3DA2DBE-30A8-2341-B5B3-919179C8B8BC}"/>
+    <workbookView xWindow="2295" yWindow="2295" windowWidth="21600" windowHeight="11385" xr2:uid="{D3DA2DBE-30A8-2341-B5B3-919179C8B8BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="14">
   <si>
     <t>Balsa_Wood_Stringer_ID</t>
   </si>
@@ -71,12 +71,6 @@
     <t>Final PreTest Weight - Grams</t>
   </si>
   <si>
-    <t>Test Orientation</t>
-  </si>
-  <si>
-    <t>Blue on Top</t>
-  </si>
-  <si>
     <t>Test File Name - 0.03 in/second</t>
   </si>
   <si>
@@ -84,9 +78,6 @@
   </si>
   <si>
     <t>Specimen Failed in Foam Layers and balsawood sheared unexpectedly</t>
-  </si>
-  <si>
-    <t>Blue on Bottom</t>
   </si>
 </sst>
 </file>
@@ -441,21 +432,22 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.6640625" customWidth="1"/>
-    <col min="3" max="3" width="28.6640625" customWidth="1"/>
-    <col min="4" max="4" width="33.1640625" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" customWidth="1"/>
-    <col min="6" max="6" width="33.1640625" customWidth="1"/>
-    <col min="7" max="7" width="71.1640625" customWidth="1"/>
-    <col min="8" max="8" width="31.83203125" customWidth="1"/>
+    <col min="1" max="1" width="31.625" customWidth="1"/>
+    <col min="2" max="2" width="25.25" customWidth="1"/>
+    <col min="3" max="3" width="28.625" customWidth="1"/>
+    <col min="4" max="4" width="33.125" customWidth="1"/>
+    <col min="5" max="5" width="15.625" customWidth="1"/>
+    <col min="6" max="6" width="33.125" customWidth="1"/>
+    <col min="7" max="7" width="71.125" customWidth="1"/>
+    <col min="8" max="8" width="31.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -469,13 +461,10 @@
         <v>10</v>
       </c>
       <c r="E1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
         <v>11</v>
-      </c>
-      <c r="G1" t="s">
-        <v>13</v>
       </c>
       <c r="H1" t="s">
         <v>5</v>
@@ -487,7 +476,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>101</v>
       </c>
@@ -503,9 +492,6 @@
       <c r="E2">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
       <c r="H2">
         <v>201</v>
       </c>
@@ -516,7 +502,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>102</v>
       </c>
@@ -532,9 +518,6 @@
       <c r="E3">
         <v>4</v>
       </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
       <c r="H3">
         <v>202</v>
       </c>
@@ -542,7 +525,7 @@
         <v>124.2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>103</v>
       </c>
@@ -558,9 +541,6 @@
       <c r="E4">
         <v>5</v>
       </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
       <c r="H4">
         <v>203</v>
       </c>
@@ -568,7 +548,7 @@
         <v>126.5</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>104</v>
       </c>
@@ -584,9 +564,6 @@
       <c r="E5">
         <v>6</v>
       </c>
-      <c r="F5" t="s">
-        <v>12</v>
-      </c>
       <c r="H5">
         <v>204</v>
       </c>
@@ -594,7 +571,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>105</v>
       </c>
@@ -610,9 +587,6 @@
       <c r="E6">
         <v>7</v>
       </c>
-      <c r="F6" t="s">
-        <v>12</v>
-      </c>
       <c r="H6">
         <v>205</v>
       </c>
@@ -623,7 +597,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>106</v>
       </c>
@@ -639,14 +613,11 @@
       <c r="E7">
         <v>8</v>
       </c>
-      <c r="F7" t="s">
-        <v>12</v>
-      </c>
       <c r="G7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>107</v>
       </c>
@@ -662,11 +633,8 @@
       <c r="E8">
         <v>9</v>
       </c>
-      <c r="F8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>108</v>
       </c>
@@ -682,11 +650,8 @@
       <c r="E9">
         <v>10</v>
       </c>
-      <c r="F9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>109</v>
       </c>
@@ -702,11 +667,8 @@
       <c r="E10">
         <v>11</v>
       </c>
-      <c r="F10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>110</v>
       </c>
@@ -722,11 +684,8 @@
       <c r="E11">
         <v>12</v>
       </c>
-      <c r="F11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>111</v>
       </c>
@@ -742,11 +701,8 @@
       <c r="E12">
         <v>14</v>
       </c>
-      <c r="F12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>112</v>
       </c>
@@ -762,11 +718,8 @@
       <c r="E13">
         <v>15</v>
       </c>
-      <c r="F13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>113</v>
       </c>
@@ -782,11 +735,8 @@
       <c r="E14">
         <v>16</v>
       </c>
-      <c r="F14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>114</v>
       </c>
@@ -802,11 +752,8 @@
       <c r="E15">
         <v>17</v>
       </c>
-      <c r="F15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>115</v>
       </c>
@@ -822,11 +769,8 @@
       <c r="E16">
         <v>18</v>
       </c>
-      <c r="F16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>116</v>
       </c>
@@ -842,11 +786,8 @@
       <c r="E17">
         <v>19</v>
       </c>
-      <c r="F17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>117</v>
       </c>
@@ -862,11 +803,8 @@
       <c r="E18">
         <v>20</v>
       </c>
-      <c r="F18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>118</v>
       </c>
@@ -882,11 +820,8 @@
       <c r="E19">
         <v>21</v>
       </c>
-      <c r="F19" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>119</v>
       </c>
@@ -902,11 +837,8 @@
       <c r="E20">
         <v>22</v>
       </c>
-      <c r="F20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>120</v>
       </c>
@@ -921,9 +853,6 @@
       </c>
       <c r="E21">
         <v>23</v>
-      </c>
-      <c r="F21" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>